<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2024-12-24.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2024-12-24.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2024-12-24.xlsx
@@ -520,6 +520,9 @@
       <c r="C11" t="str">
         <v>418_松虫草白_scabiosa white_undefined_1bunch</v>
       </c>
+      <c r="F11" t="str">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -581,7 +584,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>010135331020660</v>
+        <v>0101353310206628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>